<commit_message>
Modify Projektstrukturplan: renumber IDs
</commit_message>
<xml_diff>
--- a/doc/Projektstrukturplan.xlsx
+++ b/doc/Projektstrukturplan.xlsx
@@ -15,6 +15,7 @@
   <definedNames>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">Tabelle1!$A$1:$R$13</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">Tabelle1!$A$1:$R$13</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0" vbProcedure="false">Tabelle1!$A$1:$R$13</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -590,8 +591,8 @@
   </sheetPr>
   <dimension ref="A1:R17"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="50" zoomScaleNormal="50" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P17" activeCellId="0" sqref="P17:Q17"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Q11" activeCellId="0" sqref="Q11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -648,29 +649,41 @@
       <c r="A3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="4"/>
+      <c r="B3" s="4" t="n">
+        <v>1</v>
+      </c>
       <c r="D3" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="4"/>
+      <c r="E3" s="4" t="n">
+        <v>2</v>
+      </c>
       <c r="G3" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="H3" s="4"/>
+      <c r="H3" s="4" t="n">
+        <v>3</v>
+      </c>
       <c r="J3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="K3" s="4"/>
+      <c r="K3" s="4" t="n">
+        <v>4</v>
+      </c>
       <c r="L3" s="5"/>
       <c r="M3" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="N3" s="4"/>
+      <c r="N3" s="4" t="n">
+        <v>5</v>
+      </c>
       <c r="O3" s="5"/>
       <c r="P3" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="Q3" s="4"/>
+      <c r="Q3" s="4" t="n">
+        <v>6</v>
+      </c>
       <c r="R3" s="5"/>
     </row>
     <row r="4" customFormat="false" ht="19.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -688,7 +701,7 @@
         <v>7</v>
       </c>
       <c r="B5" s="4" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>8</v>
@@ -697,7 +710,7 @@
         <v>9</v>
       </c>
       <c r="E5" s="4" t="n">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>8</v>
@@ -706,7 +719,7 @@
         <v>10</v>
       </c>
       <c r="H5" s="4" t="n">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>8</v>
@@ -715,7 +728,7 @@
         <v>11</v>
       </c>
       <c r="K5" s="4" t="n">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="L5" s="5" t="s">
         <v>12</v>
@@ -724,7 +737,7 @@
         <v>13</v>
       </c>
       <c r="N5" s="4" t="n">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="O5" s="5" t="s">
         <v>14</v>
@@ -733,7 +746,7 @@
         <v>15</v>
       </c>
       <c r="Q5" s="4" t="n">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="R5" s="5" t="s">
         <v>14</v>
@@ -750,7 +763,7 @@
         <v>16</v>
       </c>
       <c r="B7" s="4" t="n">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>8</v>
@@ -759,7 +772,7 @@
         <v>17</v>
       </c>
       <c r="E7" s="4" t="n">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>8</v>
@@ -768,7 +781,7 @@
         <v>18</v>
       </c>
       <c r="H7" s="4" t="n">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>19</v>
@@ -777,7 +790,7 @@
         <v>20</v>
       </c>
       <c r="K7" s="4" t="n">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="L7" s="5" t="s">
         <v>19</v>
@@ -786,7 +799,7 @@
         <v>21</v>
       </c>
       <c r="N7" s="4" t="n">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="O7" s="5" t="s">
         <v>22</v>
@@ -795,7 +808,7 @@
         <v>23</v>
       </c>
       <c r="Q7" s="4" t="n">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="R7" s="5" t="s">
         <v>14</v>
@@ -811,7 +824,7 @@
         <v>24</v>
       </c>
       <c r="B9" s="4" t="n">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>8</v>
@@ -820,7 +833,7 @@
         <v>25</v>
       </c>
       <c r="E9" s="4" t="n">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>19</v>
@@ -829,7 +842,7 @@
         <v>26</v>
       </c>
       <c r="H9" s="4" t="n">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>27</v>
@@ -838,7 +851,7 @@
         <v>21</v>
       </c>
       <c r="K9" s="4" t="n">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="L9" s="5" t="s">
         <v>22</v>
@@ -850,7 +863,7 @@
         <v>28</v>
       </c>
       <c r="Q9" s="4" t="n">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="R9" s="5" t="s">
         <v>29</v>
@@ -877,7 +890,7 @@
         <v>30</v>
       </c>
       <c r="E11" s="4" t="n">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>31</v>
@@ -886,7 +899,7 @@
         <v>32</v>
       </c>
       <c r="H11" s="4" t="n">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="I11" s="1" t="s">
         <v>19</v>
@@ -895,7 +908,7 @@
         <v>33</v>
       </c>
       <c r="K11" s="4" t="n">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="L11" s="5" t="s">
         <v>31</v>
@@ -931,7 +944,7 @@
         <v>34</v>
       </c>
       <c r="H13" s="4" t="n">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="I13" s="1" t="s">
         <v>31</v>
@@ -940,7 +953,7 @@
         <v>35</v>
       </c>
       <c r="K13" s="4" t="n">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="L13" s="5" t="s">
         <v>14</v>
@@ -1012,8 +1025,8 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="50" zoomScaleNormal="50" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="P17:Q17 A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1038,8 +1051,8 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="50" zoomScaleNormal="50" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="P17:Q17 A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>